<commit_message>
added doc files (ER)
added ER diagram, adapted protocol
</commit_message>
<xml_diff>
--- a/doku/Protokoll.xlsx
+++ b/doku/Protokoll.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Pascal Lagger</t>
   </si>
@@ -43,23 +43,68 @@
 </t>
   </si>
   <si>
-    <t>Recherche API für Übersetzungen, Ziele für 1.Iteration</t>
-  </si>
-  <si>
-    <t>Webservice Grundaufbau, Ziele für 1.Iteration</t>
-  </si>
-  <si>
-    <t>Datenmodell, Ziele für 1.Iteration, Recherche Responsive WPF</t>
-  </si>
-  <si>
-    <t>Datenmodell, Ziele für 1.Iteration, Dokumentation, Formulierung der Grundidee</t>
+    <t>01.12.2017 - 14.12.2017</t>
+  </si>
+  <si>
+    <t>22.09.2017 - 5.10.2017</t>
+  </si>
+  <si>
+    <t>06.10.2017 - 19.10.2017</t>
+  </si>
+  <si>
+    <t>20.10.2017 - 02.11.2017</t>
+  </si>
+  <si>
+    <t>03.11.2017 - 16.11.2017</t>
+  </si>
+  <si>
+    <t>17.11.2017 - 30.11.2017</t>
+  </si>
+  <si>
+    <t>1.Sprint</t>
+  </si>
+  <si>
+    <t>2.Sprint</t>
+  </si>
+  <si>
+    <t>3.Sprint</t>
+  </si>
+  <si>
+    <t>4.Sprint</t>
+  </si>
+  <si>
+    <t>Datenmodell, Ziele für 1.Sprint, Recherche Responsive WPF</t>
+  </si>
+  <si>
+    <t>Datenmodell, Ziele für 1.Sprint, Dokumentation, Formulierung der Grundidee</t>
+  </si>
+  <si>
+    <t>Recherche API für Übersetzungen, Ziele für 1.Sprint</t>
+  </si>
+  <si>
+    <t>Webservice Grundaufbau, Ziele für 1.Sprint</t>
+  </si>
+  <si>
+    <t>15.12.2017 - 28.12.2017</t>
+  </si>
+  <si>
+    <t>29.12.2017 - 11.01.2018</t>
+  </si>
+  <si>
+    <t>5.Sprint</t>
+  </si>
+  <si>
+    <t>12.01.2018 - 25.01.2018</t>
+  </si>
+  <si>
+    <t>26.01.2018 - 08.01.2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +128,21 @@
     </font>
     <font>
       <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -98,7 +158,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -134,41 +194,143 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -484,236 +646,466 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF3A162-F92B-4F97-A9AF-116D8FA1D71E}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.77734375" style="1" customWidth="1"/>
-    <col min="3" max="5" width="30.21875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="19.6640625" style="4" customWidth="1"/>
+    <col min="2" max="11" width="39.77734375" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="11.5546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B1" s="2">
-        <v>43007</v>
-      </c>
-      <c r="C1" s="2">
-        <v>43008</v>
-      </c>
-      <c r="D1" s="2">
-        <v>43009</v>
-      </c>
-      <c r="E1" s="2">
-        <v>43010</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="1" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="73.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="B3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:11" s="12" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" spans="1:5" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+    </row>
+    <row r="5" spans="1:11" ht="73.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="B5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="1:5" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="B6" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+    </row>
+    <row r="7" spans="1:11" ht="73.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="B7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="1:5" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+    </row>
+    <row r="9" spans="1:11" ht="73.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="B9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+    </row>
+    <row r="11" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B7">
+  <mergeCells count="5">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:E4">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:E6">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:E8">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:E10">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:G4">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6:G6">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8:G8">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10:G10">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:I4">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -725,7 +1117,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5">
+  <conditionalFormatting sqref="H6:I6">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -737,7 +1129,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
+  <conditionalFormatting sqref="H8:I8">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -749,7 +1141,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:E3">
+  <conditionalFormatting sqref="H10:I10">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4:K4">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -761,7 +1165,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:E5">
+  <conditionalFormatting sqref="J6:K6">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -773,7 +1177,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:E7">
+  <conditionalFormatting sqref="J8:K8">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -785,7 +1189,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:E9">
+  <conditionalFormatting sqref="J10:K10">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
edited protocol; removed DailyScrums
edited protocol: added progress to first sprint and description for second sprint part
removed daily scrums due to documentation method change
</commit_message>
<xml_diff>
--- a/doku/Protokoll.xlsx
+++ b/doku/Protokoll.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pascal\Documents\BSD\Project\doku\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Herbst\Desktop\5BHIFS\BSD\Project\doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{0FA65BFB-0ECE-44D7-B986-EC09806CAB30}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048"/>
   </bookViews>
   <sheets>
     <sheet name="Protokoll" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Pascal Lagger</t>
   </si>
@@ -101,12 +101,15 @@
   </si>
   <si>
     <t>Anpassung Datenmodell, Recherche Webtechnologien, Einplegung des Datenmodells, Erstellen von Triggern etc.</t>
+  </si>
+  <si>
+    <t>Fortsetzung: Recherche Responsive WPF; GUI Mockups für C#-Anwendung</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -648,12 +651,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF3A162-F92B-4F97-A9AF-116D8FA1D71E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C7" sqref="C7"/>
+      <selection pane="topRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -726,7 +729,9 @@
       <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -740,8 +745,12 @@
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
+      <c r="B4" s="10">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0.2</v>
+      </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
@@ -1214,7 +1223,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475061E9-3DDB-49A5-A8A6-6FB9242CB73A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
updated strings and added Sprinttargets
</commit_message>
<xml_diff>
--- a/doku/Protokoll.xlsx
+++ b/doku/Protokoll.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shark333\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\5BHIFS\BSD\BSD_Project\doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Pascal Lagger</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>Webservice Recherche, Ziele für 1.Sprint</t>
+  </si>
+  <si>
+    <t>Anforderung von Key für die API, erste MockUps und Grunddesign AndroidApp</t>
   </si>
 </sst>
 </file>
@@ -293,10 +296,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -334,18 +343,6 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -665,336 +662,342 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C11" sqref="C11"/>
+      <selection pane="topRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" style="2" customWidth="1"/>
-    <col min="2" max="11" width="39.7109375" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="11.5703125" style="2"/>
+    <col min="1" max="1" width="19.7109375" style="4" customWidth="1"/>
+    <col min="2" max="11" width="39.7109375" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="11.5703125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="18" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="18" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="18" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="19"/>
-      <c r="J1" s="18" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="19"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="73.900000000000006" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:11" s="10" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:11" s="12" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="10">
         <v>1</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="11">
         <v>0.2</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:11" ht="73.900000000000006" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="10">
         <v>1</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="11">
         <v>0.3</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
     </row>
     <row r="7" spans="1:11" ht="73.900000000000006" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
+      <c r="C7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
     </row>
     <row r="8" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
+      <c r="B8" s="10">
+        <v>1</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
     </row>
     <row r="9" spans="1:11" ht="73.900000000000006" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="10">
         <v>1</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="11">
         <v>0.15</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
updated protocol, function description
</commit_message>
<xml_diff>
--- a/doku/Protokoll.xlsx
+++ b/doku/Protokoll.xlsx
@@ -103,7 +103,7 @@
     <t>Anpassung Datenmodell, Recherche Webtechnologien, Einplegung des Datenmodells, Erstellen von Triggern etc.</t>
   </si>
   <si>
-    <t>Fortsetzung: Recherche Responsive WPF; GUI Mockups für C#-Anwendung</t>
+    <t>zusätzliche Recherche responsive WPF, Finalisierung des Datenmodells, Detaillierte Erhebung der Funktionen jeder einzelnen Schiene</t>
   </si>
 </sst>
 </file>
@@ -656,7 +656,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C5" sqref="C5"/>
+      <selection pane="topRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -749,7 +749,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="11">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>

</xml_diff>